<commit_message>
BD Terminada y correciones Formulario
</commit_message>
<xml_diff>
--- a/Normalizacion.xlsx
+++ b/Normalizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agush\Desktop\UTN\2020\PAV1\Practico\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FA5479-0A45-4510-9A01-3D0D6EC67958}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1700087B-7B0F-4ADE-B7A1-3F7F90F6D02C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{AE72A06D-F57D-4A5B-9DEF-355B884F3503}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="58">
   <si>
     <t>Planta</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>IdEstado</t>
+  </si>
+  <si>
+    <t>Monto</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -405,36 +408,39 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,7 +764,7 @@
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +803,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -832,7 +838,7 @@
       <c r="P2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="42" t="s">
+      <c r="Q2" s="30" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="4" t="s">
@@ -841,8 +847,8 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="4"/>
@@ -1022,13 +1028,13 @@
         <v>26</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="37" t="s">
+      <c r="O8" s="33" t="s">
         <v>1</v>
       </c>
       <c r="P8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="35" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="4"/>
@@ -1055,11 +1061,11 @@
         <v>32</v>
       </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="38"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="31"/>
+      <c r="Q9" s="36"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
@@ -1088,12 +1094,12 @@
       <c r="N10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="38"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="17" t="s">
         <v>37</v>
       </c>
       <c r="Q10" s="4"/>
-      <c r="R10" s="30" t="s">
+      <c r="R10" s="39" t="s">
         <v>5</v>
       </c>
       <c r="S10" s="4"/>
@@ -1114,7 +1120,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="31" t="s">
         <v>1</v>
       </c>
       <c r="I11" s="20" t="s">
@@ -1127,12 +1133,12 @@
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="38"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="17" t="s">
         <v>36</v>
       </c>
       <c r="Q11" s="4"/>
-      <c r="R11" s="31"/>
+      <c r="R11" s="36"/>
       <c r="S11" s="4"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1147,7 +1153,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="41"/>
+      <c r="H12" s="32"/>
       <c r="I12" s="20" t="s">
         <v>28</v>
       </c>
@@ -1278,7 +1284,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="31" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1287,7 +1293,7 @@
       <c r="D17" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="37" t="s">
+      <c r="E17" s="33" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="17" t="s">
@@ -1301,39 +1307,39 @@
         <v>49</v>
       </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="42" t="s">
+      <c r="M17" s="30" t="s">
         <v>1</v>
       </c>
       <c r="N17" s="17" t="s">
         <v>14</v>
       </c>
       <c r="O17" s="4"/>
-      <c r="P17" s="37" t="s">
+      <c r="P17" s="33" t="s">
         <v>1</v>
       </c>
       <c r="Q17" s="17" t="s">
         <v>36</v>
       </c>
       <c r="R17" s="4"/>
-      <c r="S17" s="39" t="s">
+      <c r="S17" s="38" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="41"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="24" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="38"/>
+      <c r="E18" s="34"/>
       <c r="F18" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="37" t="s">
         <v>1</v>
       </c>
       <c r="K18" s="28" t="s">
@@ -1345,12 +1351,12 @@
         <v>10</v>
       </c>
       <c r="O18" s="4"/>
-      <c r="P18" s="38"/>
+      <c r="P18" s="34"/>
       <c r="Q18" s="17" t="s">
         <v>37</v>
       </c>
       <c r="R18" s="4"/>
-      <c r="S18" s="31"/>
+      <c r="S18" s="36"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -1363,16 +1369,16 @@
       <c r="F19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="35" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="35"/>
+      <c r="J19" s="37"/>
       <c r="K19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="32" t="s">
+      <c r="L19" s="40" t="s">
         <v>5</v>
       </c>
       <c r="M19" s="4"/>
@@ -1398,14 +1404,14 @@
       <c r="F20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="31"/>
+      <c r="G20" s="36"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="35"/>
+      <c r="J20" s="37"/>
       <c r="K20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="32"/>
+      <c r="L20" s="40"/>
       <c r="M20" s="4"/>
       <c r="N20" s="17" t="s">
         <v>26</v>
@@ -1434,12 +1440,12 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="35"/>
+      <c r="J21" s="37"/>
       <c r="K21" s="17" t="s">
         <v>50</v>
       </c>
       <c r="L21" s="4"/>
-      <c r="M21" s="36" t="s">
+      <c r="M21" s="42" t="s">
         <v>5</v>
       </c>
       <c r="N21" s="17" t="s">
@@ -1469,12 +1475,12 @@
         <v>5</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="35"/>
+      <c r="J22" s="37"/>
       <c r="K22" s="17" t="s">
         <v>46</v>
       </c>
       <c r="L22" s="4"/>
-      <c r="M22" s="36"/>
+      <c r="M22" s="42"/>
       <c r="N22" s="17" t="s">
         <v>25</v>
       </c>
@@ -1494,23 +1500,25 @@
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="35"/>
+      <c r="J23" s="37"/>
       <c r="K23" s="3" t="s">
         <v>2</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="36"/>
+      <c r="M23" s="42"/>
       <c r="N23" s="17" t="s">
         <v>13</v>
       </c>
       <c r="O23" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="P23" s="35" t="s">
+      <c r="P23" s="37" t="s">
         <v>1</v>
       </c>
       <c r="Q23" s="17" t="s">
@@ -1531,7 +1539,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="35"/>
+      <c r="J24" s="37"/>
       <c r="K24" s="17" t="s">
         <v>38</v>
       </c>
@@ -1543,12 +1551,12 @@
       <c r="O24" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="P24" s="35"/>
+      <c r="P24" s="37"/>
       <c r="Q24" s="17" t="s">
         <v>46</v>
       </c>
       <c r="R24" s="28"/>
-      <c r="S24" s="33" t="s">
+      <c r="S24" s="35" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1574,12 +1582,12 @@
         <v>53</v>
       </c>
       <c r="O25" s="4"/>
-      <c r="P25" s="35"/>
+      <c r="P25" s="37"/>
       <c r="Q25" s="3" t="s">
         <v>2</v>
       </c>
       <c r="R25" s="4"/>
-      <c r="S25" s="34"/>
+      <c r="S25" s="41"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
@@ -1862,11 +1870,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="G19:G20"/>
     <mergeCell ref="J18:J24"/>
     <mergeCell ref="P17:P18"/>
     <mergeCell ref="S17:S18"/>
@@ -1877,6 +1880,11 @@
     <mergeCell ref="S24:S25"/>
     <mergeCell ref="P23:P25"/>
     <mergeCell ref="M21:M23"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="G19:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Back end transaccion y Bd nueva
</commit_message>
<xml_diff>
--- a/Normalizacion.xlsx
+++ b/Normalizacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agush\Desktop\UTN\2020\PAV1\Practico\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1700087B-7B0F-4ADE-B7A1-3F7F90F6D02C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF1116-EA1F-425F-A3BB-ACC991392105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{AE72A06D-F57D-4A5B-9DEF-355B884F3503}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="63">
   <si>
     <t>Planta</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>Monto</t>
+  </si>
+  <si>
+    <t>Id_Detalle</t>
+  </si>
+  <si>
+    <t>TipoFactura</t>
+  </si>
+  <si>
+    <t>NroFactura</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Id_Producto</t>
   </si>
 </sst>
 </file>
@@ -363,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -398,7 +413,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -411,7 +425,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -426,21 +454,21 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -761,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C91712B-056B-4FBD-9C83-74C466677C82}">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +831,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -838,7 +866,7 @@
       <c r="P2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="R2" s="4" t="s">
@@ -847,8 +875,8 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="27" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="4"/>
@@ -1009,7 +1037,7 @@
       <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="4"/>
@@ -1028,13 +1056,13 @@
         <v>26</v>
       </c>
       <c r="N8" s="4"/>
-      <c r="O8" s="33" t="s">
+      <c r="O8" s="38" t="s">
         <v>1</v>
       </c>
       <c r="P8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="35" t="s">
+      <c r="Q8" s="40" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="4"/>
@@ -1049,7 +1077,7 @@
       <c r="F9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="4"/>
@@ -1061,11 +1089,11 @@
         <v>32</v>
       </c>
       <c r="N9" s="4"/>
-      <c r="O9" s="34"/>
+      <c r="O9" s="39"/>
       <c r="P9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="Q9" s="36"/>
+      <c r="Q9" s="41"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
     </row>
@@ -1091,15 +1119,15 @@
       <c r="M10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="O10" s="34"/>
+      <c r="N10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="39"/>
       <c r="P10" s="17" t="s">
         <v>37</v>
       </c>
       <c r="Q10" s="4"/>
-      <c r="R10" s="39" t="s">
+      <c r="R10" s="44" t="s">
         <v>5</v>
       </c>
       <c r="S10" s="4"/>
@@ -1120,7 +1148,7 @@
         <v>18</v>
       </c>
       <c r="G11" s="4"/>
-      <c r="H11" s="31" t="s">
+      <c r="H11" s="35" t="s">
         <v>1</v>
       </c>
       <c r="I11" s="20" t="s">
@@ -1133,12 +1161,12 @@
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="34"/>
+      <c r="O11" s="39"/>
       <c r="P11" s="17" t="s">
         <v>36</v>
       </c>
       <c r="Q11" s="4"/>
-      <c r="R11" s="36"/>
+      <c r="R11" s="41"/>
       <c r="S11" s="4"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1153,7 +1181,7 @@
         <v>10</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="32"/>
+      <c r="H12" s="37"/>
       <c r="I12" s="20" t="s">
         <v>28</v>
       </c>
@@ -1207,14 +1235,14 @@
       <c r="C14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="22" t="s">
         <v>5</v>
       </c>
       <c r="H14" s="4"/>
@@ -1276,30 +1304,32 @@
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="21" t="s">
+      <c r="Q16" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="R16" s="22"/>
+      <c r="R16" s="34"/>
       <c r="S16" s="4"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="35" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="33" t="s">
+      <c r="D17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="38" t="s">
         <v>1</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="22" t="s">
+        <v>5</v>
+      </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1307,42 +1337,40 @@
         <v>49</v>
       </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="30" t="s">
+      <c r="M17" s="29" t="s">
         <v>1</v>
       </c>
       <c r="N17" s="17" t="s">
         <v>14</v>
       </c>
       <c r="O17" s="4"/>
-      <c r="P17" s="33" t="s">
+      <c r="P17" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="R17" s="4"/>
-      <c r="S17" s="38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q17" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="24" t="s">
+      <c r="B18" s="37"/>
+      <c r="C18" s="23" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="34"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="37" t="s">
+      <c r="J18" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="28" t="s">
+      <c r="K18" s="27" t="s">
         <v>14</v>
       </c>
       <c r="L18" s="4"/>
@@ -1351,14 +1379,16 @@
         <v>10</v>
       </c>
       <c r="O18" s="4"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="R18" s="4"/>
-      <c r="S18" s="36"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P18" s="47"/>
+      <c r="Q18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="R18" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="S18" s="14"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
@@ -1369,16 +1399,16 @@
       <c r="F19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="40" t="s">
         <v>5</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="37"/>
+      <c r="J19" s="42"/>
       <c r="K19" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="40" t="s">
+      <c r="L19" s="45" t="s">
         <v>5</v>
       </c>
       <c r="M19" s="4"/>
@@ -1386,14 +1416,14 @@
         <v>41</v>
       </c>
       <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P19" s="47"/>
+      <c r="Q19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="R19" s="46"/>
+      <c r="S19" s="14"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
@@ -1404,27 +1434,29 @@
       <c r="F20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="36"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="37"/>
+      <c r="J20" s="42"/>
       <c r="K20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="L20" s="40"/>
+      <c r="L20" s="45"/>
       <c r="M20" s="4"/>
       <c r="N20" s="17" t="s">
         <v>26</v>
       </c>
       <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P20" s="47"/>
+      <c r="Q20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="R20" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="S20" s="14"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
@@ -1440,24 +1472,28 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="37"/>
+      <c r="J21" s="42"/>
       <c r="K21" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="42" t="s">
-        <v>5</v>
-      </c>
+      <c r="L21" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="M21" s="25"/>
       <c r="N21" s="17" t="s">
         <v>42</v>
       </c>
       <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="R21" s="22" t="s">
+        <v>5</v>
+      </c>
       <c r="S21" s="4"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
@@ -1471,28 +1507,26 @@
         <v>39</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="24" t="s">
         <v>5</v>
       </c>
       <c r="I22" s="4"/>
-      <c r="J22" s="37"/>
+      <c r="J22" s="42"/>
       <c r="K22" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="42"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="25"/>
       <c r="N22" s="17" t="s">
         <v>25</v>
       </c>
       <c r="O22" s="4"/>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
@@ -1506,31 +1540,26 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="37"/>
+      <c r="J23" s="42"/>
       <c r="K23" s="3" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="L23" s="4"/>
-      <c r="M23" s="42"/>
+      <c r="M23" s="25"/>
       <c r="N23" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="O23" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="P23" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="R23" s="4"/>
-      <c r="S23" s="26"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O23" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>10</v>
       </c>
       <c r="D24" s="4"/>
@@ -1539,31 +1568,23 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="17" t="s">
-        <v>38</v>
+      <c r="J24" s="43"/>
+      <c r="K24" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="O24" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="R24" s="28"/>
-      <c r="S24" s="35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O24" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="26" t="s">
         <v>41</v>
       </c>
       <c r="D25" s="4"/>
@@ -1574,65 +1595,57 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="L25" s="28"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="L25" s="27"/>
+      <c r="M25" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="N25" s="28" t="s">
         <v>53</v>
       </c>
       <c r="O25" s="4"/>
-      <c r="P25" s="37"/>
-      <c r="Q25" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R25" s="4"/>
-      <c r="S25" s="41"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>54</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+      <c r="F26" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="29" t="s">
-        <v>52</v>
-      </c>
+      <c r="K26" s="28"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="23" t="s">
-        <v>5</v>
-      </c>
+      <c r="M26" s="12"/>
       <c r="N26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O26" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="R26" s="4"/>
-      <c r="S26" s="12"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O26" s="22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+      <c r="D27" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
@@ -1642,22 +1655,16 @@
       <c r="M27" s="4"/>
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="R27" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="S27" s="4"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="F28" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
@@ -1669,10 +1676,13 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
+      <c r="R28" s="21" t="s">
+        <v>45</v>
+      </c>
       <c r="S28" s="4"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T28" s="4"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1689,11 +1699,16 @@
       <c r="N29" s="12"/>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
+      <c r="Q29" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>18</v>
+      </c>
       <c r="S29" s="4"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T29" s="25"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1710,11 +1725,16 @@
       <c r="N30" s="12"/>
       <c r="O30" s="12"/>
       <c r="P30" s="12"/>
-      <c r="Q30" s="4"/>
-      <c r="R30" s="4"/>
-      <c r="S30" s="4"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q30" s="42"/>
+      <c r="R30" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="S30" s="27"/>
+      <c r="T30" s="31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1731,11 +1751,14 @@
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="17" t="s">
+        <v>47</v>
+      </c>
       <c r="S31" s="4"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T31" s="32"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1753,10 +1776,15 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R32" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S32" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="T32" s="12"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1773,11 +1801,10 @@
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q33" s="12"/>
+      <c r="T33" s="4"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
@@ -1790,7 +1817,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
@@ -1803,7 +1830,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
@@ -1816,7 +1843,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
@@ -1829,7 +1856,7 @@
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
@@ -1842,7 +1869,7 @@
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -1855,7 +1882,7 @@
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
@@ -1869,17 +1896,15 @@
       <c r="R40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="13">
+    <mergeCell ref="Q29:Q30"/>
+    <mergeCell ref="R18:R19"/>
     <mergeCell ref="J18:J24"/>
-    <mergeCell ref="P17:P18"/>
-    <mergeCell ref="S17:S18"/>
     <mergeCell ref="O8:O11"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="L19:L20"/>
-    <mergeCell ref="S24:S25"/>
-    <mergeCell ref="P23:P25"/>
-    <mergeCell ref="M21:M23"/>
+    <mergeCell ref="L21:L22"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B17:B18"/>

</xml_diff>